<commit_message>
Removed Random Mobile Numbers
</commit_message>
<xml_diff>
--- a/Original_Data/CustomFormatting.xlsx
+++ b/Original_Data/CustomFormatting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\Documents\GitHub_Excel\Original_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D8061FF-36B0-4C65-8FA9-87632CEBA364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D283CCD9-1C1C-4750-8636-FAD6184D0F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{27E4171C-0AAB-4F46-82E6-7837F22D7C86}"/>
   </bookViews>
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1479,8 +1479,7 @@
         <v>590</v>
       </c>
       <c r="C2" s="5">
-        <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(1000000000,(10000000000)-1)</f>
-        <v>2959366854</v>
+        <v>4759462429</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1494,8 +1493,7 @@
         <v>231</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3433373024</v>
+        <v>3111843265</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1509,8 +1507,7 @@
         <v>386</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6832852815</v>
+        <v>3007723039</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1524,8 +1521,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1683302183</v>
+        <v>1530049582</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1539,8 +1535,7 @@
         <v>258</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6283152051</v>
+        <v>9584299252</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1554,8 +1549,7 @@
         <v>975</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4228390711</v>
+        <v>7720819933</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1569,8 +1563,7 @@
         <v>1-869</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9848739422</v>
+        <v>3447612857</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1584,8 +1577,7 @@
         <v>599</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>7118464645</v>
+        <v>9486032302</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1599,8 +1591,7 @@
         <v>595</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1467748396</v>
+        <v>8062846356</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1614,8 +1605,7 @@
         <v>246</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4792427139</v>
+        <v>2279190723</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1629,8 +1619,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4804938479</v>
+        <v>8371665677</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1644,8 +1633,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1970928785</v>
+        <v>5265926213</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>

</xml_diff>